<commit_message>
se agrego la placa en el ticket de salida y que los cajeros vean la lista
</commit_message>
<xml_diff>
--- a/public/lavadas.xlsx
+++ b/public/lavadas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,51 +464,219 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>asas1239</t>
+          <t>JKJ3865</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>toyota</t>
+          <t>NISSAN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-05-26 18:53 PM</t>
+          <t>2024-06-13 13:00 PM</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-31 19:22:00</t>
+          <t>2024-06-18 23:00:00</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>edicion</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dead3625</t>
+          <t>JPK2456</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>chevy</t>
+          <t>HONDA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-05-26 19:25 PM</t>
+          <t>2024-06-13 13:09 PM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-05-30 19:36:00</t>
-        </is>
-      </c>
+          <t>2024-06-18 23:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>JLA3831</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HONDA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-06-13 14:07 PM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-06-11 22:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>294XUJ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>VOLKSWAGEN</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-06-13 16:13 PM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-06-17 18:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>G19BMM</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MAZDA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-06-13 18:57 PM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>JSJ2237</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MINI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-06-13 21:21 PM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JNR1775</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NISSAN</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-06-14 02:45 AM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-06-21 19:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>JUB9526</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NISSAN</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-06-14 03:04 AM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-06-18 23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ALEJANDRA VANESSA JIMENEZ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JLY1080</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MITSUBISHI</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-06-14 03:13 AM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HWF430A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PEUGEOT</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-06-14 03:58 AM</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
se agregaron los cambios para el pensionado
</commit_message>
<xml_diff>
--- a/public/lavadas.xlsx
+++ b/public/lavadas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,222 +461,46 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>JKJ3865</t>
+          <t>prueba0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NISSAN</t>
+          <t>honda</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-06-13 13:00 PM</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-06-18 23:00:00</t>
-        </is>
-      </c>
+          <t>2024-09-10 09:49 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>JPK2456</t>
+          <t>7163gmk</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HONDA</t>
+          <t>honda</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-06-13 13:09 PM</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-06-18 23:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>JLA3831</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>HONDA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-06-13 14:07 PM</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-06-11 22:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>294XUJ</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>VOLKSWAGEN</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-06-13 16:13 PM</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024-06-17 18:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>G19BMM</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>MAZDA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024-06-13 18:57 PM</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>JSJ2237</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MINI</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024-06-13 21:21 PM</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>JNR1775</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NISSAN</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2024-06-14 02:45 AM</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2024-06-21 19:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>JUB9526</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NISSAN</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2024-06-14 03:04 AM</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2024-06-18 23:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ALEJANDRA VANESSA JIMENEZ</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JLY1080</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>MITSUBISHI</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2024-06-14 03:13 AM</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>HWF430A</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>PEUGEOT</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2024-06-14 03:58 AM</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>2024-09-10 09:56 AM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
se agregaron lo de las lavadas
</commit_message>
<xml_diff>
--- a/public/lavadas.xlsx
+++ b/public/lavadas.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$E$8</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -425,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,48 +463,161 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>prueba0</t>
+          <t>JRS6561</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>SEAT</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-09-10 07:19 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-09-12 23:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PYR831E</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TOYOTA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:56 AM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-09-13 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23N050</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MAZDA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-09-10 09:10 AM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-09-13 13:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NAP068A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NISSAN</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:02 AM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-09-14 10:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>JSL2080</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MAZDA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-09-10 09:18 AM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2024-09-15 13:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C22BHG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>AUDI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-09-10 08:53 AM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2024-09-15 20:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ADOLFO REYES AGUIRRE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>JSB4919</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>honda</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-09-10 09:49 AM</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>7163gmk</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>honda</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024-09-10 09:56 AM</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-09-11 17:41 PM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E8"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>